<commit_message>
modules and sub modules added in communicator/database/Structure.xml
</commit_message>
<xml_diff>
--- a/database/Structure.xlsx
+++ b/database/Structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="138">
   <si>
     <t>Container</t>
   </si>
@@ -63,9 +63,6 @@
     <t>vehicleDeviceId</t>
   </si>
   <si>
-    <t>VehicleDevice</t>
-  </si>
-  <si>
     <t>taggingDate</t>
   </si>
   <si>
@@ -256,13 +253,194 @@
   </si>
   <si>
     <t>altitude</t>
+  </si>
+  <si>
+    <t>VDevice</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Sub-Module</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Dependency, RnD</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Tag Registration.</t>
+  </si>
+  <si>
+    <t>1) Web Application Showing Tags
+2) Desktop Application For Reading Tag</t>
+  </si>
+  <si>
+    <t>Container Registration.</t>
+  </si>
+  <si>
+    <t>Web Application For Registering Container</t>
+  </si>
+  <si>
+    <t>Where To Get Container Information ?</t>
+  </si>
+  <si>
+    <t>Vehicle Registration.</t>
+  </si>
+  <si>
+    <t>Web Application For Registering Vehicle</t>
+  </si>
+  <si>
+    <t>Where To Get Vehicle Information ?</t>
+  </si>
+  <si>
+    <t>Vehicle Device Registration.</t>
+  </si>
+  <si>
+    <t>Where To Get Device Id ?</t>
+  </si>
+  <si>
+    <t>Base Station Registration</t>
+  </si>
+  <si>
+    <t>Web Application For Registering Base Station</t>
+  </si>
+  <si>
+    <t>Where To Get Base Station Id ?</t>
+  </si>
+  <si>
+    <t>Fixed RFID Reader Registration.</t>
+  </si>
+  <si>
+    <t>Web Application For Registering RFID Fixed Reader</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Creating Container Block</t>
+  </si>
+  <si>
+    <t>Web Application</t>
+  </si>
+  <si>
+    <t>Where to get Lat-Long for creating Container Block ?</t>
+  </si>
+  <si>
+    <t>Creating Container Area Within A Block For A Container</t>
+  </si>
+  <si>
+    <t>Where to get Lat-Long for creating Container Area ?</t>
+  </si>
+  <si>
+    <t>Creating Fixed Reader Location</t>
+  </si>
+  <si>
+    <t>Middleware Configuration</t>
+  </si>
+  <si>
+    <t>Web Application For Middleware Configuration Setting</t>
+  </si>
+  <si>
+    <t>How to Assign Static IP To FIXED RFID Reader?</t>
+  </si>
+  <si>
+    <t>Base Station Configuration</t>
+  </si>
+  <si>
+    <t>Web Application For Base Station Configuration Settings</t>
+  </si>
+  <si>
+    <t>How to Save Mqtt Host and IP In Base Station Device ?</t>
+  </si>
+  <si>
+    <t>Application for Mapping Tag ID with Container.</t>
+  </si>
+  <si>
+    <t>Desktop Application For Mapping</t>
+  </si>
+  <si>
+    <t>Application for Mapping Device ID with Vehicle.</t>
+  </si>
+  <si>
+    <t>Web Application For Mapping</t>
+  </si>
+  <si>
+    <t>Application for Mapping Fixed Reader with Location of Yard.</t>
+  </si>
+  <si>
+    <t>Data Acquisition</t>
+  </si>
+  <si>
+    <t>Acquirig GPS Data from Base Station Device communicating over MQTT Broker.</t>
+  </si>
+  <si>
+    <t>Consumer Service For Receiving Data</t>
+  </si>
+  <si>
+    <t>Acquirig Fixed RFID Reader Notification From Middleware over MQTT Broker.</t>
+  </si>
+  <si>
+    <t>1) Pushing MQTT Notification In Middleware
+2) Consumer Service For Receiving Data In WebApplication</t>
+  </si>
+  <si>
+    <t>Acquirig Movement Data from The Fixed RFID Reader</t>
+  </si>
+  <si>
+    <t>1) Web Services For Receiving Data For Middleware.
+2) Calling the webservice from Middleware</t>
+  </si>
+  <si>
+    <t>Middleware</t>
+  </si>
+  <si>
+    <t>Receiving and filtering the bulk data from fixed reader.</t>
+  </si>
+  <si>
+    <t>Middleware Application</t>
+  </si>
+  <si>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t>Creating User And Authentication.</t>
+  </si>
+  <si>
+    <t>1) Web Application For User
+2) Login Authentication</t>
+  </si>
+  <si>
+    <t>Middleware Connection Status</t>
+  </si>
+  <si>
+    <t>Base Station Connection Status</t>
+  </si>
+  <si>
+    <t>Fixed RFID Reader Connection Status</t>
+  </si>
+  <si>
+    <t>Container Movement By Fixed RFID Reader</t>
+  </si>
+  <si>
+    <t>Map View Of Container Location</t>
+  </si>
+  <si>
+    <t>Data Processing And Visualization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,16 +456,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -347,14 +569,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,12 +659,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69:F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,19 +996,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -717,17 +1018,17 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -743,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>5</v>
@@ -752,54 +1053,54 @@
         <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -821,79 +1122,79 @@
         <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="5"/>
+      <c r="B22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>8</v>
@@ -903,164 +1204,164 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
+      <c r="B26" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J27" s="7"/>
-      <c r="K27" s="8"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="4"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="B30" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="H34" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
+      <c r="B34" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="H34" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="K35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>6</v>
@@ -1068,177 +1369,177 @@
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="5"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="19"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="M39" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+      <c r="B42" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+      <c r="B46" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+      <c r="B50" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="5"/>
+      <c r="B54" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="19"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>5</v>
@@ -1247,30 +1548,30 @@
         <v>1</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
+      <c r="B58" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>14</v>
@@ -1285,19 +1586,19 @@
         <v>1</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H59" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I59" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="J59" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>6</v>
@@ -1329,12 +1630,354 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="63.5703125" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="23">
+        <v>1</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="23">
+        <v>2</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="23">
+        <v>3</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="13">
+        <v>4</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="13">
+        <v>5</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="20">
+        <v>6</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>